<commit_message>
Rename reporoot from Ordnungssysteme to Ordnungssystem for all XLSX templates:
The plural spelling was introduced by mistake, and makes no sense.
</commit_message>
<xml_diff>
--- a/opengever/bundle/tests/assets/basic_repository.xlsx
+++ b/opengever/bundle/tests/assets/basic_repository.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Work/development/opengever.core/opengever/bundle/tests/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukasgraf/Plone/buildouts/opengever/og-zgschmieden/opengever/bundle/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BA48A5-BD48-F24F-AFB9-A16B0D17C0A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A311CC1-9A3C-5640-9BC8-91F55CF7F2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="108">
   <si>
     <t>reference_number</t>
   </si>
@@ -436,9 +436,6 @@
   </si>
   <si>
     <t>og_demo-ftw_users</t>
-  </si>
-  <si>
-    <t>Ordnungssysteme</t>
   </si>
   <si>
     <t>Système de classement</t>
@@ -1463,7 +1460,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1529,7 +1526,7 @@
         <v>65</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>60</v>
@@ -1594,7 +1591,7 @@
         <v>63</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>55</v>
@@ -1659,7 +1656,7 @@
         <v>41</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="44" t="s">
         <v>2</v>
@@ -1716,13 +1713,13 @@
     <row r="6" spans="1:21" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>96</v>
-      </c>
       <c r="D6" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
@@ -1801,7 +1798,7 @@
         <v>81</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="24" t="s">
@@ -1829,7 +1826,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="24" t="s">
@@ -1842,13 +1839,13 @@
         <v>25</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L9" s="24">
         <v>150</v>
@@ -1867,7 +1864,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="24" t="s">
@@ -1895,7 +1892,7 @@
         <v>84</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="24" t="s">
@@ -1925,7 +1922,7 @@
         <v>85</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="24" t="s">
@@ -1953,7 +1950,7 @@
         <v>86</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="24" t="s">

</xml_diff>